<commit_message>
Updated grout injection property definitions
</commit_message>
<xml_diff>
--- a/Dictionaries/DIGGSGroutInjectionPropertyDefinitions.xlsx
+++ b/Dictionaries/DIGGSGroutInjectionPropertyDefinitions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dponti/GitHub/diggs-schema/Dictionaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E2A1D7-150F-E745-85CE-588C29A64B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{114AAF14-3530-B84B-8389-14517ACB3FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15820" yWindow="2560" windowWidth="41460" windowHeight="28240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="42600" windowHeight="27620" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DictionaryName" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="137">
   <si>
     <t>Code</t>
   </si>
@@ -150,18 +149,9 @@
     <t>take</t>
   </si>
   <si>
-    <t>depth</t>
-  </si>
-  <si>
     <t>drilling_index</t>
   </si>
   <si>
-    <t>drilling_speed</t>
-  </si>
-  <si>
-    <t>fluid_1_pressure</t>
-  </si>
-  <si>
     <t>fluid_2_flow</t>
   </si>
   <si>
@@ -186,9 +176,6 @@
     <t>micro_motion_volume</t>
   </si>
   <si>
-    <t>pull_speed</t>
-  </si>
-  <si>
     <t>rotary_pressure</t>
   </si>
   <si>
@@ -201,18 +188,9 @@
     <t>torque</t>
   </si>
   <si>
-    <t>fluid_1_temperature</t>
-  </si>
-  <si>
-    <t>fluid_1_flow</t>
-  </si>
-  <si>
     <t>line_loss</t>
   </si>
   <si>
-    <t>apparent lugeon valuie</t>
-  </si>
-  <si>
     <t>column pressure</t>
   </si>
   <si>
@@ -222,9 +200,6 @@
     <t>drilling index</t>
   </si>
   <si>
-    <t>drilling speed</t>
-  </si>
-  <si>
     <t>effective pressure</t>
   </si>
   <si>
@@ -285,9 +260,6 @@
     <t>packer pressure</t>
   </si>
   <si>
-    <t>pull speed</t>
-  </si>
-  <si>
     <t>rotary pressure</t>
   </si>
   <si>
@@ -309,9 +281,6 @@
     <t>volume per time</t>
   </si>
   <si>
-    <t>??</t>
-  </si>
-  <si>
     <t>volume</t>
   </si>
   <si>
@@ -324,54 +293,33 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>Depth of the monitor at a specific time instance</t>
-  </si>
-  <si>
     <t>/diggs:Diggs/diggs:constructionActivity/diggs:BoreholeGroutingActivity/diggs:groutStage/diggs:GroutStage</t>
   </si>
   <si>
     <t>/diggs:Diggs/diggs:constructionActivity/diggs:BoreholeGroutingActivity/diggs:continuousGrouting/diggs:ContinuousGrouting</t>
   </si>
   <si>
-    <t>Advance rate of the monitor while drilling downward</t>
-  </si>
-  <si>
     <t>Amount of time since start of an injection period</t>
   </si>
   <si>
-    <t>Pressure reading of fluid 1 during injection</t>
-  </si>
-  <si>
-    <t>Temperature of fluid 1</t>
-  </si>
-  <si>
     <t>Pressure reading of fluid 2 during injection</t>
   </si>
   <si>
     <t>Temperature of fluid 2</t>
   </si>
   <si>
-    <t>Pressure measured at the base of the column</t>
-  </si>
-  <si>
     <t>Pressure measured at the gauge</t>
   </si>
   <si>
     <t>Rate of flow of the grout component during injection</t>
   </si>
   <si>
-    <t>Rate of flow of the fluid 1 component (either water or air) as defined in the instance</t>
-  </si>
-  <si>
     <t>Rate of flow of the fluid 2 component (either water or air) as defined in the instance</t>
   </si>
   <si>
     <t>grout specific gravity</t>
   </si>
   <si>
-    <t>Pressure reading of the grout (not sure wher this is supposed to be measured)… Used for jet and other grouting</t>
-  </si>
-  <si>
     <t>Temperature of the grout component</t>
   </si>
   <si>
@@ -381,12 +329,6 @@
     <t>Volume of grout injected during the present time interval</t>
   </si>
   <si>
-    <t>Pressure measured at the header pipe</t>
-  </si>
-  <si>
-    <t>Used for grout stage injections - how different from other pressures?</t>
-  </si>
-  <si>
     <t>Flow rate of grout measured by Micro Motion branded sensor</t>
   </si>
   <si>
@@ -396,15 +338,6 @@
     <t>Identifer for the grout mix used</t>
   </si>
   <si>
-    <t>Lift rate of the monitor while grouting</t>
-  </si>
-  <si>
-    <t>Rotational velocity of the monitor</t>
-  </si>
-  <si>
-    <t>energy per mass</t>
-  </si>
-  <si>
     <t>Pressure times flow divided by lift rate. Pressure can be measured at the pump or at the drill rig and is not measured at the nozzle. Lift rate is average uplift distance per unit time. Pressure at the pump can be affected by line type, size, and distance to the rig for constant applied pressure. The energy of the air is usually negligible in this calculation, but does contribute significantly to column diameter. This parameter can be graphed to quickly check jetting records and can be correlated to diameter for all other aspects (especially number of fluids) staying constant during the test program.</t>
   </si>
   <si>
@@ -412,6 +345,108 @@
   </si>
   <si>
     <t>Total volume of grout injected</t>
+  </si>
+  <si>
+    <t>Hydraulic system pressure to spin the drill steel</t>
+  </si>
+  <si>
+    <t>Downward hydraulic pressure of the drill (not at the bit)</t>
+  </si>
+  <si>
+    <t>energy per meter</t>
+  </si>
+  <si>
+    <t>Measure of bit performance calculated using a number of dimensionless parameters</t>
+  </si>
+  <si>
+    <t>Rotational force of the drill</t>
+  </si>
+  <si>
+    <t>Downward force of the drill</t>
+  </si>
+  <si>
+    <t>apparent lugeon value</t>
+  </si>
+  <si>
+    <t>Pressure measured at the header</t>
+  </si>
+  <si>
+    <t>pressure per length</t>
+  </si>
+  <si>
+    <t>Pressure lost through the line</t>
+  </si>
+  <si>
+    <t>Pressure within the packer</t>
+  </si>
+  <si>
+    <t>Pressure felt at injection point (pressure at pump - line loss)</t>
+  </si>
+  <si>
+    <t>Pressure reading of the grout</t>
+  </si>
+  <si>
+    <t>Pressure of the grout being injected (often used for grout stage injections)</t>
+  </si>
+  <si>
+    <t>Calculated hydrostatic pressure on borehole wall</t>
+  </si>
+  <si>
+    <t>blade_rotation_number</t>
+  </si>
+  <si>
+    <t>blade rotation number</t>
+  </si>
+  <si>
+    <t>fluid_3_flow</t>
+  </si>
+  <si>
+    <t>fluid_3_pressure</t>
+  </si>
+  <si>
+    <t>fluid_3_temperature</t>
+  </si>
+  <si>
+    <t>Rate of flow of the fluid 3 component (either water or air) as defined in the instance</t>
+  </si>
+  <si>
+    <t>Pressure reading of fluid 3 during injection</t>
+  </si>
+  <si>
+    <t>Temperature of fluid 3</t>
+  </si>
+  <si>
+    <t>advance_rate</t>
+  </si>
+  <si>
+    <t>advance rate</t>
+  </si>
+  <si>
+    <t>withdrawal_rate</t>
+  </si>
+  <si>
+    <t>Advance rate of the monitor, drill bit, or cutting tool while drilling downward, also known as drilling speed</t>
+  </si>
+  <si>
+    <t>Lift rate of the monitor or cutting tool while grouting, also known as the pull speed</t>
+  </si>
+  <si>
+    <t>measured_distance</t>
+  </si>
+  <si>
+    <t>measured distance</t>
+  </si>
+  <si>
+    <t>Measured depth of the monitor or cutting tool, or the measured distance from the start of a grout trench, at a specific time instance</t>
+  </si>
+  <si>
+    <t>For soil mixing, the total number of mixing blades passing for 1 m of shaft/tool movement</t>
+  </si>
+  <si>
+    <t>Measure of permeability via in-situ pressure testing</t>
+  </si>
+  <si>
+    <t>Rotational velocity of the monitor or cutting tool</t>
   </si>
 </sst>
 </file>
@@ -493,12 +528,14 @@
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -510,10 +547,8 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="4">
@@ -587,7 +622,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -639,15 +674,17 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="9" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1199,8 +1236,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H132"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1241,143 +1278,152 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" s="11" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="str">
-        <f>IF(ISNA(VLOOKUP(C2,AssociatedElements!B$2:B3019,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(C2,AssociatedElements!B$2:B3036,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B2" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>126</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="12"/>
+        <v>127</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>129</v>
+      </c>
       <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="str">
-        <f>IF(ISNA(VLOOKUP(C3,AssociatedElements!B$2:B3020,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(C3,AssociatedElements!B$2:B3019,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B3" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>104</v>
+        <v>109</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>135</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="str">
-        <f>IF(ISNA(VLOOKUP(C4,AssociatedElements!B$2:B3018,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(C4,AssociatedElements!B$2:B3056,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>6</v>
-      </c>
+      <c r="C4" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="str">
-        <f>IF(ISNA(VLOOKUP(C5,AssociatedElements!B$2:B3034,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(C5,AssociatedElements!B$2:B3020,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>95</v>
+        <v>51</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>117</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="str">
-        <f>IF(ISNA(VLOOKUP(C6,AssociatedElements!B$2:B3035,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(C6,AssociatedElements!B$2:B3018,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F6" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="G6" s="26" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="str">
-        <f>IF(ISNA(VLOOKUP(C7,AssociatedElements!B$2:B3036,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(C7,AssociatedElements!B$2:B3035,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="F7" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>18</v>
+      <c r="G7" s="12" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -1392,7 +1438,10 @@
         <v>26</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>62</v>
+        <v>54</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>114</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>4</v>
@@ -1413,10 +1462,10 @@
         <v>27</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>4</v>
@@ -1427,44 +1476,44 @@
     </row>
     <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="str">
-        <f>IF(ISNA(VLOOKUP(C10,AssociatedElements!B$2:B3038,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(C10,AssociatedElements!B$2:B3041,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B10" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="str">
-        <f>IF(ISNA(VLOOKUP(C11,AssociatedElements!B$2:B3039,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(C11,AssociatedElements!B$2:B3042,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>4</v>
@@ -1475,20 +1524,20 @@
     </row>
     <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="str">
-        <f>IF(ISNA(VLOOKUP(C12,AssociatedElements!B$2:B3040,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(C12,AssociatedElements!B$2:B3043,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B12" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>4</v>
@@ -1499,44 +1548,44 @@
     </row>
     <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="str">
-        <f>IF(ISNA(VLOOKUP(C13,AssociatedElements!B$2:B3041,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(C13,AssociatedElements!B$2:B3038,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B13" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>41</v>
+        <v>120</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="str">
-        <f>IF(ISNA(VLOOKUP(C14,AssociatedElements!B$2:B3042,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(C14,AssociatedElements!B$2:B3039,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B14" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>42</v>
+        <v>121</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>102</v>
+        <v>124</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>4</v>
@@ -1547,20 +1596,20 @@
     </row>
     <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="str">
-        <f>IF(ISNA(VLOOKUP(C15,AssociatedElements!B$2:B3043,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(C15,AssociatedElements!B$2:B3040,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B15" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>43</v>
+        <v>122</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>103</v>
+        <v>125</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>4</v>
@@ -1581,10 +1630,10 @@
         <v>28</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>4</v>
@@ -1602,22 +1651,22 @@
         <v>21</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="str">
         <f>IF(ISNA(VLOOKUP(C18,AssociatedElements!B$2:B3045,1,FALSE)),"Not used","")</f>
         <v/>
@@ -1626,13 +1675,13 @@
         <v>21</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E18" s="26" t="s">
-        <v>110</v>
+        <v>64</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>115</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>4</v>
@@ -1653,15 +1702,15 @@
         <v>29</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G19" s="26" t="s">
+      <c r="G19" s="12" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1677,10 +1726,10 @@
         <v>30</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>4</v>
@@ -1698,19 +1747,19 @@
         <v>21</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -1725,10 +1774,10 @@
         <v>31</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E22" s="26" t="s">
-        <v>114</v>
+        <v>67</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>110</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>4</v>
@@ -1749,10 +1798,10 @@
         <v>32</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E23" s="26" t="s">
-        <v>115</v>
+        <v>68</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>116</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>4</v>
@@ -1770,136 +1819,142 @@
         <v>21</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>77</v>
+        <v>69</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>112</v>
       </c>
       <c r="F24" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G24" s="26" t="s">
-        <v>90</v>
+      <c r="G24" s="12" t="s">
+        <v>111</v>
       </c>
       <c r="H24" s="11"/>
     </row>
-    <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="str">
-        <f>IF(ISNA(VLOOKUP(C25,AssociatedElements!B$2:B3048,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(C25,AssociatedElements!B$2:B3034,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B25" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>47</v>
+        <v>131</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>89</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="str">
-        <f>IF(ISNA(VLOOKUP(C26,AssociatedElements!B$2:B3049,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(C26,AssociatedElements!B$2:B3048,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B26" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="str">
-        <f>IF(ISNA(VLOOKUP(C27,AssociatedElements!B$2:B3030,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(C27,AssociatedElements!B$2:B3049,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B27" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="str">
-        <f>IF(ISNA(VLOOKUP(C28,AssociatedElements!B$2:B3031,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(C28,AssociatedElements!B$2:B3030,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B28" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="H28" s="11"/>
+      <c r="C28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="str">
-        <f>IF(ISNA(VLOOKUP(C29,AssociatedElements!B$2:B3050,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(C29,AssociatedElements!B$2:B3031,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B29" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>82</v>
+      <c r="C29" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>73</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="F29" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F29" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G29" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="G29" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H29" s="11"/>
     </row>
     <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="16" t="str">
@@ -1910,10 +1965,13 @@
         <v>21</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>83</v>
+        <v>74</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>103</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>4</v>
@@ -1931,19 +1989,19 @@
         <v>21</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="119" x14ac:dyDescent="0.2">
@@ -1955,19 +2013,19 @@
         <v>21</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G32" s="26" t="s">
-        <v>121</v>
+      <c r="G32" s="12" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -1982,13 +2040,13 @@
         <v>35</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>14</v>
@@ -2007,16 +2065,16 @@
         <v>36</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -2033,6 +2091,9 @@
       <c r="D35" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="E35" s="12" t="s">
+        <v>108</v>
+      </c>
       <c r="F35" s="3" t="s">
         <v>4</v>
       </c>
@@ -2049,25 +2110,44 @@
         <v>21</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>107</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="str">
-        <f>IF(ISNA(VLOOKUP(C37,AssociatedElements!B$2:B3056,1,FALSE)),"Not used","")</f>
-        <v>Not used</v>
-      </c>
-      <c r="D37" s="4"/>
-      <c r="G37" s="4"/>
+        <f>IF(ISNA(VLOOKUP(C37,AssociatedElements!B$2:B3050,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="str">
@@ -2857,7 +2937,7 @@
   <sheetViews>
     <sheetView zoomScale="106" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2885,10 +2965,10 @@
         <v/>
       </c>
       <c r="B2" s="3" t="s">
-        <v>24</v>
+        <v>126</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2897,10 +2977,10 @@
         <v/>
       </c>
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2908,11 +2988,11 @@
         <f>IF(ISNA(VLOOKUP(B4,Definitions!C$2:C$2003,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>97</v>
+      <c r="B4" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2921,10 +3001,10 @@
         <v/>
       </c>
       <c r="B5" s="3" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2932,11 +3012,11 @@
         <f>IF(ISNA(VLOOKUP(B6,Definitions!C$2:C$2003,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>38</v>
+      <c r="B6" s="11" t="s">
+        <v>23</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2945,10 +3025,10 @@
         <v/>
       </c>
       <c r="B7" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2960,7 +3040,7 @@
         <v>26</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2972,7 +3052,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2984,7 +3064,7 @@
         <v>27</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -2993,10 +3073,10 @@
         <v/>
       </c>
       <c r="B11" s="3" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -3005,10 +3085,10 @@
         <v/>
       </c>
       <c r="B12" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -3017,10 +3097,10 @@
         <v/>
       </c>
       <c r="B13" s="3" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -3029,10 +3109,10 @@
         <v/>
       </c>
       <c r="B14" s="3" t="s">
-        <v>41</v>
+        <v>120</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -3041,10 +3121,10 @@
         <v/>
       </c>
       <c r="B15" s="3" t="s">
-        <v>42</v>
+        <v>121</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -3053,10 +3133,10 @@
         <v/>
       </c>
       <c r="B16" s="3" t="s">
-        <v>43</v>
+        <v>122</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -3068,7 +3148,7 @@
         <v>28</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -3077,10 +3157,10 @@
         <v/>
       </c>
       <c r="B18" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -3089,10 +3169,10 @@
         <v/>
       </c>
       <c r="B19" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -3101,10 +3181,10 @@
         <v/>
       </c>
       <c r="B20" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -3113,10 +3193,10 @@
         <v/>
       </c>
       <c r="B21" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -3128,7 +3208,7 @@
         <v>29</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -3139,8 +3219,8 @@
       <c r="B23" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="27" t="s">
-        <v>97</v>
+      <c r="C23" s="25" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -3152,7 +3232,7 @@
         <v>30</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -3163,8 +3243,8 @@
       <c r="B25" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="27" t="s">
-        <v>97</v>
+      <c r="C25" s="25" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -3173,10 +3253,10 @@
         <v/>
       </c>
       <c r="B26" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="27" t="s">
-        <v>97</v>
+        <v>43</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -3187,8 +3267,8 @@
       <c r="B27" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="27" t="s">
-        <v>97</v>
+      <c r="C27" s="25" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -3200,7 +3280,7 @@
         <v>32</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -3209,10 +3289,10 @@
         <v/>
       </c>
       <c r="B29" s="11" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -3221,10 +3301,10 @@
         <v/>
       </c>
       <c r="B30" s="3" t="s">
-        <v>47</v>
+        <v>131</v>
       </c>
       <c r="C30" s="27" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -3233,10 +3313,10 @@
         <v/>
       </c>
       <c r="B31" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C31" s="27" t="s">
-        <v>97</v>
+        <v>44</v>
+      </c>
+      <c r="C31" s="25" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -3245,10 +3325,10 @@
         <v/>
       </c>
       <c r="B32" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>96</v>
+        <v>45</v>
+      </c>
+      <c r="C32" s="26" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -3256,11 +3336,11 @@
         <f>IF(ISNA(VLOOKUP(B33,Definitions!C$2:C$2003,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B33" s="11" t="s">
-        <v>34</v>
+      <c r="B33" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -3268,11 +3348,11 @@
         <f>IF(ISNA(VLOOKUP(B34,Definitions!C$2:C$2003,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="27" t="s">
-        <v>97</v>
+      <c r="B34" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="31" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -3281,10 +3361,10 @@
         <v/>
       </c>
       <c r="B35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C35" s="27" t="s">
-        <v>97</v>
+        <v>46</v>
+      </c>
+      <c r="C35" s="25" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -3293,10 +3373,10 @@
         <v/>
       </c>
       <c r="B36" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C36" s="27" t="s">
-        <v>97</v>
+        <v>47</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -3305,10 +3385,10 @@
         <v/>
       </c>
       <c r="B37" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C37" s="27" t="s">
-        <v>97</v>
+        <v>48</v>
+      </c>
+      <c r="C37" s="25" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -3320,7 +3400,7 @@
         <v>35</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -3331,8 +3411,8 @@
       <c r="B39" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="28" t="s">
-        <v>97</v>
+      <c r="C39" s="26" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -3343,8 +3423,8 @@
       <c r="B40" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C40" s="29" t="s">
-        <v>96</v>
+      <c r="C40" s="27" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -3355,8 +3435,8 @@
       <c r="B41" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="27" t="s">
-        <v>97</v>
+      <c r="C41" s="25" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -3367,8 +3447,8 @@
       <c r="B42" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C42" s="27" t="s">
-        <v>97</v>
+      <c r="C42" s="25" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -3377,19 +3457,23 @@
         <v/>
       </c>
       <c r="B43" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C43" s="27" t="s">
-        <v>97</v>
+        <v>49</v>
+      </c>
+      <c r="C43" s="25" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="str">
         <f>IF(ISNA(VLOOKUP(B44,Definitions!C$2:C$2003,1,FALSE)),"Not listed","")</f>
-        <v>Not listed</v>
-      </c>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
+        <v/>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C44" s="25" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="str">

</xml_diff>